<commit_message>
Added dSide column to all sheets, so this can be brought in along with other position information.
</commit_message>
<xml_diff>
--- a/Data/RawData/YPE_Data/YPE_10_MountRaymond/Digital Data_YPE10/YPE_PILAdata_Plot_10.xlsx
+++ b/Data/RawData/YPE_Data/YPE_10_MountRaymond/Digital Data_YPE10/YPE_PILAdata_Plot_10.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="QWdLiQpyVWwhum4V4G7I4VhkJOjw/TqMinIMAgHwJH8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="OpSLpkZHE3EFDVyIGG798Lww504H7vU+xwdUq9SJsHU="/>
     </ext>
   </extLst>
 </workbook>
@@ -865,7 +865,7 @@
         <v>50.0</v>
       </c>
       <c r="Q2" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R2" s="4">
         <v>22.0</v>
@@ -1053,7 +1053,7 @@
         <v>50.0</v>
       </c>
       <c r="Q3" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R3" s="4">
         <v>22.0</v>
@@ -1241,7 +1241,7 @@
         <v>50.0</v>
       </c>
       <c r="Q4" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R4" s="4">
         <v>22.0</v>
@@ -1429,7 +1429,7 @@
         <v>50.0</v>
       </c>
       <c r="Q5" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R5" s="4">
         <v>22.0</v>
@@ -1617,7 +1617,7 @@
         <v>50.0</v>
       </c>
       <c r="Q6" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R6" s="4">
         <v>22.0</v>
@@ -1805,7 +1805,7 @@
         <v>50.0</v>
       </c>
       <c r="Q7" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R7" s="4">
         <v>22.0</v>
@@ -1993,7 +1993,7 @@
         <v>50.0</v>
       </c>
       <c r="Q8" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R8" s="4">
         <v>22.0</v>
@@ -2181,7 +2181,7 @@
         <v>50.0</v>
       </c>
       <c r="Q9" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R9" s="4">
         <v>22.0</v>
@@ -2369,7 +2369,7 @@
         <v>50.0</v>
       </c>
       <c r="Q10" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R10" s="4">
         <v>22.0</v>
@@ -2557,7 +2557,7 @@
         <v>50.0</v>
       </c>
       <c r="Q11" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R11" s="4">
         <v>22.0</v>
@@ -2745,7 +2745,7 @@
         <v>50.0</v>
       </c>
       <c r="Q12" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R12" s="4">
         <v>22.0</v>
@@ -2930,7 +2930,7 @@
         <v>50.0</v>
       </c>
       <c r="Q13" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R13" s="4">
         <v>22.0</v>
@@ -3118,7 +3118,7 @@
         <v>50.0</v>
       </c>
       <c r="Q14" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R14" s="4">
         <v>22.0</v>
@@ -3306,7 +3306,7 @@
         <v>50.0</v>
       </c>
       <c r="Q15" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R15" s="4">
         <v>22.0</v>
@@ -3494,7 +3494,7 @@
         <v>50.0</v>
       </c>
       <c r="Q16" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R16" s="4">
         <v>22.0</v>
@@ -3682,7 +3682,7 @@
         <v>50.0</v>
       </c>
       <c r="Q17" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R17" s="4">
         <v>22.0</v>
@@ -3870,7 +3870,7 @@
         <v>50.0</v>
       </c>
       <c r="Q18" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R18" s="4">
         <v>22.0</v>
@@ -4058,7 +4058,7 @@
         <v>50.0</v>
       </c>
       <c r="Q19" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R19" s="4">
         <v>22.0</v>
@@ -4246,7 +4246,7 @@
         <v>50.0</v>
       </c>
       <c r="Q20" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R20" s="4">
         <v>22.0</v>
@@ -4434,7 +4434,7 @@
         <v>50.0</v>
       </c>
       <c r="Q21" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R21" s="4">
         <v>22.0</v>
@@ -4622,7 +4622,7 @@
         <v>50.0</v>
       </c>
       <c r="Q22" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R22" s="4">
         <v>22.0</v>
@@ -4810,7 +4810,7 @@
         <v>50.0</v>
       </c>
       <c r="Q23" s="4">
-        <v>342.5</v>
+        <v>330.0</v>
       </c>
       <c r="R23" s="4">
         <v>22.0</v>

</xml_diff>